<commit_message>
Feat:Add SaleManager domain and Create fileUpload API
</commit_message>
<xml_diff>
--- a/src/main/resources/매출액 업로드 첨부파일.xlsx
+++ b/src/main/resources/매출액 업로드 첨부파일.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wmf2fkrh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wmf2fkrh\git\BootCamp\sales-data-collection-backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{033EAFA4-FC69-4ABA-BF6D-ACB08963848A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4081154-2EBA-4CC2-BF05-724E0541508A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6C7DA09F-68D5-40D4-80EC-C4CACBF3D990}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{6C7DA09F-68D5-40D4-80EC-C4CACBF3D990}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>회사명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -44,15 +44,17 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>매출일(년도)</t>
+    <t>매출액</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>매출일(월)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>매출액</t>
+    <t>영업이익</t>
+  </si>
+  <si>
+    <t>당기순이익</t>
+  </si>
+  <si>
+    <t>기준일자(년월)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -417,20 +419,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C192E75F-FDB9-46CA-9E2D-C1330A66919F}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,6 +449,9 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat:Create download api and Refactor sale domain
</commit_message>
<xml_diff>
--- a/src/main/resources/매출액 업로드 첨부파일.xlsx
+++ b/src/main/resources/매출액 업로드 첨부파일.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wmf2fkrh\git\BootCamp\sales-data-collection-backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4081154-2EBA-4CC2-BF05-724E0541508A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9773BCE1-C8A9-4EF4-874F-B00FC876CD38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{6C7DA09F-68D5-40D4-80EC-C4CACBF3D990}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="19200" windowHeight="9960" xr2:uid="{6C7DA09F-68D5-40D4-80EC-C4CACBF3D990}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>회사명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,13 +48,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>기준일자(년월)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>영업이익</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>당기순이익</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>기준일자(년월)</t>
+    <t>이메일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -62,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +79,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -96,18 +111,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -419,22 +450,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C192E75F-FDB9-46CA-9E2D-C1330A66919F}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.4140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" customWidth="1"/>
-    <col min="4" max="4" width="9.58203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.4140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.58203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.4140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,17 +474,370 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C4" s="4"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C7" s="4"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C9" s="4"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C10" s="4"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C15" s="4"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C16" s="4"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C18" s="4"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C19" s="4"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C22" s="4"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C23" s="4"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C24" s="4"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C25" s="4"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C26" s="4"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C27" s="4"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C28" s="4"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C29" s="4"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C30" s="4"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C31" s="4"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C32" s="4"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C33" s="4"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C34" s="4"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C35" s="4"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C36" s="4"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C37" s="4"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C38" s="4"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C39" s="4"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C40" s="4"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C41" s="4"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C42" s="4"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C43" s="4"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C44" s="4"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C45" s="4"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C46" s="4"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C47" s="4"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C48" s="4"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C49" s="4"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C50" s="4"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C51" s="4"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>